<commit_message>
modified : xlsx uploading
</commit_message>
<xml_diff>
--- a/app/cert_gen_sen_app_backend/certificate_data/Contact Information.xlsx
+++ b/app/cert_gen_sen_app_backend/certificate_data/Contact Information.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Timestamp</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Full Name</t>
   </si>
   <si>
+    <t>Student Id</t>
+  </si>
+  <si>
     <t>Email</t>
   </si>
   <si>
@@ -35,6 +38,9 @@
   </si>
   <si>
     <t>Siddhant Totade 1</t>
+  </si>
+  <si>
+    <t>MU19BTCSE007</t>
   </si>
   <si>
     <t>siddhanttotade.1994@gmail.com</t>
@@ -92,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -109,8 +115,17 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -119,7 +134,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -423,7 +438,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
@@ -431,12 +446,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="18.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="28.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="41.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="28.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="41.57642857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -449,14 +465,17 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
@@ -464,18 +483,21 @@
         <v>44886.88539351852</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5">
-        <v>8889428579</v>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="E2" s="4">
+        <v>25672.116071516204</v>
+      </c>
+      <c r="F2" s="1">
         <v>44886</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="4">
         <v>44887</v>
       </c>
     </row>
@@ -483,19 +505,22 @@
       <c r="A3" s="1">
         <v>44887.88539351852</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6">
         <v>8889428579</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="7">
         <v>44887</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="7">
         <v>44888</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified : new event and user added
</commit_message>
<xml_diff>
--- a/app/cert_gen_sen_app_backend/certificate_data/Contact Information.xlsx
+++ b/app/cert_gen_sen_app_backend/certificate_data/Contact Information.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Timestamp</t>
   </si>
@@ -31,31 +31,28 @@
     <t>Certificate Status</t>
   </si>
   <si>
-    <t>Siddhant Totade 1</t>
-  </si>
-  <si>
-    <t>MU19BTCSE006</t>
-  </si>
-  <si>
-    <t>siddhanttotade.1994@gmail.com</t>
+    <t>Himanshu Kashyap</t>
+  </si>
+  <si>
+    <t>MU19BTCSE017</t>
+  </si>
+  <si>
+    <t>himmu7987@gmail.com</t>
   </si>
   <si>
     <t>F</t>
   </si>
   <si>
-    <t>Siddhant Totade 2</t>
-  </si>
-  <si>
-    <t>MU19BTCSE004</t>
+    <t>Prakash Singh</t>
+  </si>
+  <si>
+    <t>MU19BTCSE002L</t>
+  </si>
+  <si>
+    <t>kshatreeya545@gmail.com</t>
   </si>
   <si>
     <t>T</t>
-  </si>
-  <si>
-    <t>Siddhant Totade 3</t>
-  </si>
-  <si>
-    <t>MU19BTCSE05</t>
   </si>
 </sst>
 </file>
@@ -113,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -121,13 +118,16 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -138,24 +138,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,7 +441,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
@@ -467,11 +449,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="18.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="28.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="28.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="14.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -487,7 +469,7 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -498,48 +480,31 @@
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>44887</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1">
-        <v>44887.88539351852</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug : .env is not working
</commit_message>
<xml_diff>
--- a/app/cert_gen_sen_app_backend/certificate_data/Contact Information.xlsx
+++ b/app/cert_gen_sen_app_backend/certificate_data/Contact Information.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Timestamp</t>
   </si>
@@ -31,28 +31,19 @@
     <t>Certificate Status</t>
   </si>
   <si>
-    <t>Himanshu Kashyap</t>
-  </si>
-  <si>
-    <t>MU19BTCSE017</t>
-  </si>
-  <si>
-    <t>himmu7987@gmail.com</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Prakash Singh</t>
-  </si>
-  <si>
-    <t>MU19BTCSE002L</t>
-  </si>
-  <si>
-    <t>kshatreeya545@gmail.com</t>
+    <t>Dr. Abhishek Bhadolia</t>
+  </si>
+  <si>
+    <t>drabhishekb@matsuniversity.ac.in</t>
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>Dr. M Sudhir Kumar</t>
+  </si>
+  <si>
+    <t>drsudhirkm@matsuniversity.ac.in</t>
   </si>
 </sst>
 </file>
@@ -110,16 +101,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -127,16 +124,19 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -449,62 +449,58 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="18.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="28.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="28.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="14.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1">
-        <v>44886.88539351852</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5">
+        <v>2002</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="4">
-        <v>44887</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2075</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>12</v>
+      <c r="E3" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>